<commit_message>
Se suben los laboratorio ajustados del primer cohorte de la materia
</commit_message>
<xml_diff>
--- a/Cohorte_1/Taller/2.13.Practical-example.Descriptive-statistics-exercise.xlsx
+++ b/Cohorte_1/Taller/2.13.Practical-example.Descriptive-statistics-exercise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Business_intelligence_analytics\Cohorte_1\Taller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583D8913-6968-415B-A6BA-F26D68C47827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90526CC4-709B-4BA9-9D48-D842C9014DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="365RE" sheetId="1" r:id="rId1"/>
@@ -25,8 +25,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'365RE'!$A$5:$AM$926</definedName>
     <definedName name="_xlchart.v1.0" hidden="1">'365RE'!$I$6:$I$272</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">'365RE'!$I$6:$I$272</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'365RE'!$I$6:$I$272</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'365RE'!$I$6:$I$272</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -2099,13 +2097,13 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4025,7 +4023,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5944,6 +5942,111 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>107539</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{852B02F8-F0D4-4B03-BC33-5A1ED922EB84}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="161925" y="885826"/>
+          <a:ext cx="6819900" cy="3384138"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>226200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>35700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>106041</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48BAC333-58CD-4C37-A5FA-CC42AFB4A69E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7055625" y="845325"/>
+          <a:ext cx="6898500" cy="3423141"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -6295,35 +6398,35 @@
       <c r="W3" s="14"/>
     </row>
     <row r="4" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="L4" s="36" t="s">
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="L4" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="M4" s="36"/>
-      <c r="N4" s="36"/>
-      <c r="O4" s="36"/>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="36"/>
-      <c r="R4" s="36"/>
-      <c r="S4" s="36"/>
-      <c r="T4" s="36"/>
-      <c r="U4" s="36"/>
-      <c r="V4" s="36"/>
-      <c r="W4" s="36"/>
-      <c r="X4" s="36"/>
-      <c r="Y4" s="36"/>
-      <c r="Z4" s="36"/>
-      <c r="AA4" s="36"/>
+      <c r="M4" s="38"/>
+      <c r="N4" s="38"/>
+      <c r="O4" s="38"/>
+      <c r="P4" s="38"/>
+      <c r="Q4" s="38"/>
+      <c r="R4" s="38"/>
+      <c r="S4" s="38"/>
+      <c r="T4" s="38"/>
+      <c r="U4" s="38"/>
+      <c r="V4" s="38"/>
+      <c r="W4" s="38"/>
+      <c r="X4" s="38"/>
+      <c r="Y4" s="38"/>
+      <c r="Z4" s="38"/>
+      <c r="AA4" s="38"/>
     </row>
     <row r="5" spans="2:27" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="30" t="s">
@@ -43793,7 +43896,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A7C1412-EA0B-443B-AF04-4E1F30BE9CF6}">
   <dimension ref="B1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -43999,8 +44102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11D6B83C-E8B8-4DA4-8E51-8D3B78A1B9E1}">
   <dimension ref="B1:J169"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y22" sqref="Y22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -44538,6 +44641,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -44587,7 +44691,7 @@
       <c r="B7" s="27" t="s">
         <v>558</v>
       </c>
-      <c r="C7" s="37">
+      <c r="C7" s="36">
         <f>+AVERAGE('365RE'!I6:I272)</f>
         <v>281171.90150112362</v>
       </c>
@@ -44600,7 +44704,7 @@
       <c r="B8" s="27" t="s">
         <v>559</v>
       </c>
-      <c r="C8" s="37">
+      <c r="C8" s="36">
         <f>+MEDIAN('365RE'!I6:I272)</f>
         <v>249075.6568</v>
       </c>
@@ -44613,7 +44717,7 @@
       <c r="B9" s="27" t="s">
         <v>560</v>
       </c>
-      <c r="C9" s="38">
+      <c r="C9" s="37">
         <f>+_xlfn.MODE.SNGL('365RE'!I6:I272)</f>
         <v>460001.25599999994</v>
       </c>
@@ -44639,7 +44743,7 @@
       <c r="B11" s="27" t="s">
         <v>562</v>
       </c>
-      <c r="C11" s="38">
+      <c r="C11" s="37">
         <f>+_xlfn.VAR.S('365RE'!I6:I272)</f>
         <v>7942217700.9209938</v>
       </c>
@@ -44652,7 +44756,7 @@
       <c r="B12" s="27" t="s">
         <v>563</v>
       </c>
-      <c r="C12" s="38">
+      <c r="C12" s="37">
         <f>+_xlfn.STDEV.S('365RE'!I6:I272)</f>
         <v>89119.120849125262</v>
       </c>

</xml_diff>